<commit_message>
Buenas Practicas - DFR
</commit_message>
<xml_diff>
--- a/Data/Output/Incidentes.xlsx
+++ b/Data/Output/Incidentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Downloads\LAL.001-master\LAL.001-master\Data\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Documents\UiPath\LAL.001\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11705435-04CD-46C9-B063-AF7F67964E30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2468BDA3-FE4D-4722-BA57-540105607DC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="1185" windowWidth="18000" windowHeight="9480" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
+    <workbookView xWindow="23880" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774D41E4-B09A-489E-A9A4-8A9E3169033C}">
-  <dimension ref="A1:D832"/>
+  <dimension ref="A1:D782"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
@@ -3569,206 +3569,6 @@
       <c r="B782" s="4"/>
       <c r="C782" s="5"/>
     </row>
-    <row r="783" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B783" s="4"/>
-      <c r="C783" s="5"/>
-    </row>
-    <row r="784" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B784" s="4"/>
-      <c r="C784" s="5"/>
-    </row>
-    <row r="785" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B785" s="4"/>
-      <c r="C785" s="5"/>
-    </row>
-    <row r="786" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B786" s="4"/>
-      <c r="C786" s="5"/>
-    </row>
-    <row r="787" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B787" s="4"/>
-      <c r="C787" s="5"/>
-    </row>
-    <row r="788" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B788" s="4"/>
-      <c r="C788" s="5"/>
-    </row>
-    <row r="789" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B789" s="4"/>
-      <c r="C789" s="5"/>
-    </row>
-    <row r="790" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B790" s="4"/>
-      <c r="C790" s="5"/>
-    </row>
-    <row r="791" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B791" s="4"/>
-      <c r="C791" s="5"/>
-    </row>
-    <row r="792" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B792" s="4"/>
-      <c r="C792" s="5"/>
-    </row>
-    <row r="793" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B793" s="4"/>
-      <c r="C793" s="5"/>
-    </row>
-    <row r="794" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B794" s="4"/>
-      <c r="C794" s="5"/>
-    </row>
-    <row r="795" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B795" s="4"/>
-      <c r="C795" s="5"/>
-    </row>
-    <row r="796" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B796" s="4"/>
-      <c r="C796" s="5"/>
-    </row>
-    <row r="797" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B797" s="4"/>
-      <c r="C797" s="5"/>
-    </row>
-    <row r="798" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B798" s="4"/>
-      <c r="C798" s="5"/>
-    </row>
-    <row r="799" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B799" s="4"/>
-      <c r="C799" s="5"/>
-    </row>
-    <row r="800" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B800" s="4"/>
-      <c r="C800" s="5"/>
-    </row>
-    <row r="801" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B801" s="4"/>
-      <c r="C801" s="5"/>
-    </row>
-    <row r="802" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B802" s="4"/>
-      <c r="C802" s="5"/>
-    </row>
-    <row r="803" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B803" s="4"/>
-      <c r="C803" s="5"/>
-    </row>
-    <row r="804" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B804" s="4"/>
-      <c r="C804" s="5"/>
-    </row>
-    <row r="805" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B805" s="4"/>
-      <c r="C805" s="5"/>
-    </row>
-    <row r="806" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B806" s="4"/>
-      <c r="C806" s="5"/>
-    </row>
-    <row r="807" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B807" s="4"/>
-      <c r="C807" s="5"/>
-    </row>
-    <row r="808" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B808" s="4"/>
-      <c r="C808" s="5"/>
-    </row>
-    <row r="809" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B809" s="4"/>
-      <c r="C809" s="5"/>
-    </row>
-    <row r="810" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B810" s="4"/>
-      <c r="C810" s="5"/>
-    </row>
-    <row r="811" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B811" s="4"/>
-      <c r="C811" s="5"/>
-    </row>
-    <row r="812" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B812" s="4"/>
-      <c r="C812" s="5"/>
-    </row>
-    <row r="813" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B813" s="4"/>
-      <c r="C813" s="5"/>
-    </row>
-    <row r="814" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B814" s="4"/>
-      <c r="C814" s="5"/>
-    </row>
-    <row r="815" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B815" s="4"/>
-      <c r="C815" s="5"/>
-    </row>
-    <row r="816" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B816" s="4"/>
-      <c r="C816" s="5"/>
-    </row>
-    <row r="817" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B817" s="4"/>
-      <c r="C817" s="5"/>
-    </row>
-    <row r="818" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B818" s="4"/>
-      <c r="C818" s="5"/>
-    </row>
-    <row r="819" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B819" s="4"/>
-      <c r="C819" s="5"/>
-    </row>
-    <row r="820" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B820" s="4"/>
-      <c r="C820" s="5"/>
-    </row>
-    <row r="821" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B821" s="4"/>
-      <c r="C821" s="5"/>
-    </row>
-    <row r="822" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B822" s="4"/>
-      <c r="C822" s="5"/>
-    </row>
-    <row r="823" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B823" s="4"/>
-      <c r="C823" s="5"/>
-    </row>
-    <row r="824" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B824" s="4"/>
-      <c r="C824" s="5"/>
-    </row>
-    <row r="825" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B825" s="4"/>
-      <c r="C825" s="5"/>
-    </row>
-    <row r="826" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B826" s="4"/>
-      <c r="C826" s="5"/>
-    </row>
-    <row r="827" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B827" s="4"/>
-      <c r="C827" s="5"/>
-    </row>
-    <row r="828" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B828" s="4"/>
-      <c r="C828" s="5"/>
-    </row>
-    <row r="829" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B829" s="4"/>
-      <c r="C829" s="5"/>
-    </row>
-    <row r="830" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B830" s="4"/>
-      <c r="C830" s="5"/>
-    </row>
-    <row r="831" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B831" s="4"/>
-      <c r="C831" s="5"/>
-    </row>
-    <row r="832" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B832" s="4"/>
-      <c r="C832" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solucion de buenas practicas
</commit_message>
<xml_diff>
--- a/Data/Output/Incidentes.xlsx
+++ b/Data/Output/Incidentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cruzl\Documents\UiPath\LAL.001\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2468BDA3-FE4D-4722-BA57-540105607DC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D618DC-D053-4268-B65F-E64D6965729C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{CD3CAB56-BE71-4485-8FBE-BEAF51E98128}"/>
   </bookViews>
@@ -415,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774D41E4-B09A-489E-A9A4-8A9E3169033C}">
-  <dimension ref="A1:D782"/>
+  <dimension ref="A1:D732"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
@@ -3369,206 +3369,6 @@
       <c r="B732" s="4"/>
       <c r="C732" s="5"/>
     </row>
-    <row r="733" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B733" s="4"/>
-      <c r="C733" s="5"/>
-    </row>
-    <row r="734" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B734" s="4"/>
-      <c r="C734" s="5"/>
-    </row>
-    <row r="735" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B735" s="4"/>
-      <c r="C735" s="5"/>
-    </row>
-    <row r="736" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B736" s="4"/>
-      <c r="C736" s="5"/>
-    </row>
-    <row r="737" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B737" s="4"/>
-      <c r="C737" s="5"/>
-    </row>
-    <row r="738" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B738" s="4"/>
-      <c r="C738" s="5"/>
-    </row>
-    <row r="739" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B739" s="4"/>
-      <c r="C739" s="5"/>
-    </row>
-    <row r="740" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B740" s="4"/>
-      <c r="C740" s="5"/>
-    </row>
-    <row r="741" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B741" s="4"/>
-      <c r="C741" s="5"/>
-    </row>
-    <row r="742" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B742" s="4"/>
-      <c r="C742" s="5"/>
-    </row>
-    <row r="743" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B743" s="4"/>
-      <c r="C743" s="5"/>
-    </row>
-    <row r="744" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B744" s="4"/>
-      <c r="C744" s="5"/>
-    </row>
-    <row r="745" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B745" s="4"/>
-      <c r="C745" s="5"/>
-    </row>
-    <row r="746" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B746" s="4"/>
-      <c r="C746" s="5"/>
-    </row>
-    <row r="747" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B747" s="4"/>
-      <c r="C747" s="5"/>
-    </row>
-    <row r="748" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B748" s="4"/>
-      <c r="C748" s="5"/>
-    </row>
-    <row r="749" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B749" s="4"/>
-      <c r="C749" s="5"/>
-    </row>
-    <row r="750" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B750" s="4"/>
-      <c r="C750" s="5"/>
-    </row>
-    <row r="751" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B751" s="4"/>
-      <c r="C751" s="5"/>
-    </row>
-    <row r="752" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B752" s="4"/>
-      <c r="C752" s="5"/>
-    </row>
-    <row r="753" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B753" s="4"/>
-      <c r="C753" s="5"/>
-    </row>
-    <row r="754" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B754" s="4"/>
-      <c r="C754" s="5"/>
-    </row>
-    <row r="755" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B755" s="4"/>
-      <c r="C755" s="5"/>
-    </row>
-    <row r="756" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B756" s="4"/>
-      <c r="C756" s="5"/>
-    </row>
-    <row r="757" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B757" s="4"/>
-      <c r="C757" s="5"/>
-    </row>
-    <row r="758" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B758" s="4"/>
-      <c r="C758" s="5"/>
-    </row>
-    <row r="759" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B759" s="4"/>
-      <c r="C759" s="5"/>
-    </row>
-    <row r="760" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B760" s="4"/>
-      <c r="C760" s="5"/>
-    </row>
-    <row r="761" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B761" s="4"/>
-      <c r="C761" s="5"/>
-    </row>
-    <row r="762" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B762" s="4"/>
-      <c r="C762" s="5"/>
-    </row>
-    <row r="763" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B763" s="4"/>
-      <c r="C763" s="5"/>
-    </row>
-    <row r="764" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B764" s="4"/>
-      <c r="C764" s="5"/>
-    </row>
-    <row r="765" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B765" s="4"/>
-      <c r="C765" s="5"/>
-    </row>
-    <row r="766" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B766" s="4"/>
-      <c r="C766" s="5"/>
-    </row>
-    <row r="767" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B767" s="4"/>
-      <c r="C767" s="5"/>
-    </row>
-    <row r="768" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B768" s="4"/>
-      <c r="C768" s="5"/>
-    </row>
-    <row r="769" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B769" s="4"/>
-      <c r="C769" s="5"/>
-    </row>
-    <row r="770" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B770" s="4"/>
-      <c r="C770" s="5"/>
-    </row>
-    <row r="771" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B771" s="4"/>
-      <c r="C771" s="5"/>
-    </row>
-    <row r="772" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B772" s="4"/>
-      <c r="C772" s="5"/>
-    </row>
-    <row r="773" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B773" s="4"/>
-      <c r="C773" s="5"/>
-    </row>
-    <row r="774" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B774" s="4"/>
-      <c r="C774" s="5"/>
-    </row>
-    <row r="775" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B775" s="4"/>
-      <c r="C775" s="5"/>
-    </row>
-    <row r="776" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B776" s="4"/>
-      <c r="C776" s="5"/>
-    </row>
-    <row r="777" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B777" s="4"/>
-      <c r="C777" s="5"/>
-    </row>
-    <row r="778" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B778" s="4"/>
-      <c r="C778" s="5"/>
-    </row>
-    <row r="779" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B779" s="4"/>
-      <c r="C779" s="5"/>
-    </row>
-    <row r="780" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B780" s="4"/>
-      <c r="C780" s="5"/>
-    </row>
-    <row r="781" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B781" s="4"/>
-      <c r="C781" s="5"/>
-    </row>
-    <row r="782" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B782" s="4"/>
-      <c r="C782" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>